<commit_message>
Applying strategy found in play-ground.html example
Still wip though as still not fully working
</commit_message>
<xml_diff>
--- a/Tutorial/static/Known_Data.xlsx
+++ b/Tutorial/static/Known_Data.xlsx
@@ -15,12 +15,12 @@
     <sheet name="SystemViewsFaultsreduced_LHR_01" sheetId="1" r:id="rId1"/>
     <sheet name="Key to data" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="99">
   <si>
     <t>Set_ID</t>
   </si>
@@ -314,6 +314,9 @@
   </si>
   <si>
     <t>Class G</t>
+  </si>
+  <si>
+    <t>Num_Class</t>
   </si>
 </sst>
 </file>
@@ -1123,14 +1126,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W413"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="18" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="19" max="23" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -1159,6 +1168,9 @@
       </c>
       <c r="H1" t="s">
         <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>98</v>
       </c>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
@@ -1198,6 +1210,9 @@
       <c r="H2">
         <v>1</v>
       </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1224,6 +1239,9 @@
       <c r="H3">
         <v>1</v>
       </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1250,6 +1268,9 @@
       <c r="H4">
         <v>1</v>
       </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1276,6 +1297,9 @@
       <c r="H5">
         <v>1</v>
       </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1302,6 +1326,9 @@
       <c r="H6">
         <v>1</v>
       </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -1328,6 +1355,9 @@
       <c r="H7">
         <v>1</v>
       </c>
+      <c r="I7">
+        <v>2</v>
+      </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -1354,6 +1384,9 @@
       <c r="H8">
         <v>1</v>
       </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -1380,6 +1413,9 @@
       <c r="H9">
         <v>1</v>
       </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -1406,6 +1442,9 @@
       <c r="H10">
         <v>1</v>
       </c>
+      <c r="I10">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -1432,6 +1471,9 @@
       <c r="H11">
         <v>1</v>
       </c>
+      <c r="I11">
+        <v>3</v>
+      </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -1458,6 +1500,9 @@
       <c r="H12">
         <v>1</v>
       </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -1484,6 +1529,9 @@
       <c r="H13">
         <v>1</v>
       </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -1510,6 +1558,9 @@
       <c r="H14">
         <v>1</v>
       </c>
+      <c r="I14">
+        <v>2</v>
+      </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -1536,6 +1587,9 @@
       <c r="H15">
         <v>1</v>
       </c>
+      <c r="I15">
+        <v>3</v>
+      </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -1562,8 +1616,11 @@
       <c r="H16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -1588,8 +1645,11 @@
       <c r="H17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -1614,8 +1674,11 @@
       <c r="H18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>37</v>
       </c>
@@ -1640,8 +1703,11 @@
       <c r="H19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -1666,8 +1732,11 @@
       <c r="H20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>37</v>
       </c>
@@ -1692,8 +1761,11 @@
       <c r="H21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>41</v>
       </c>
@@ -1718,8 +1790,11 @@
       <c r="H22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>43</v>
       </c>
@@ -1744,8 +1819,11 @@
       <c r="H23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>45</v>
       </c>
@@ -1770,8 +1848,11 @@
       <c r="H24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>47</v>
       </c>
@@ -1796,8 +1877,11 @@
       <c r="H25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>49</v>
       </c>
@@ -1822,8 +1906,11 @@
       <c r="H26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>41</v>
       </c>
@@ -1848,8 +1935,11 @@
       <c r="H27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>52</v>
       </c>
@@ -1874,8 +1964,11 @@
       <c r="H28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>52</v>
       </c>
@@ -1900,8 +1993,11 @@
       <c r="H29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I29">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>14</v>
       </c>
@@ -1926,8 +2022,11 @@
       <c r="H30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>43</v>
       </c>
@@ -1952,8 +2051,11 @@
       <c r="H31">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>43</v>
       </c>
@@ -1978,8 +2080,11 @@
       <c r="H32">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>43</v>
       </c>
@@ -2004,8 +2109,11 @@
       <c r="H33">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>43</v>
       </c>
@@ -2030,8 +2138,11 @@
       <c r="H34">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>43</v>
       </c>
@@ -2056,8 +2167,11 @@
       <c r="H35">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>43</v>
       </c>
@@ -2082,8 +2196,11 @@
       <c r="H36">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I36">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>43</v>
       </c>
@@ -2108,8 +2225,11 @@
       <c r="H37">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>23</v>
       </c>
@@ -2134,8 +2254,11 @@
       <c r="H38">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>23</v>
       </c>
@@ -2160,8 +2283,11 @@
       <c r="H39">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>23</v>
       </c>
@@ -2186,8 +2312,11 @@
       <c r="H40">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I40">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>60</v>
       </c>
@@ -2212,8 +2341,11 @@
       <c r="H41">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I41">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>62</v>
       </c>
@@ -2238,8 +2370,11 @@
       <c r="H42">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I42">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>64</v>
       </c>
@@ -2264,8 +2399,11 @@
       <c r="H43">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I43">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>66</v>
       </c>
@@ -2290,8 +2428,11 @@
       <c r="H44">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>41</v>
       </c>
@@ -2316,8 +2457,11 @@
       <c r="H45">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>68</v>
       </c>
@@ -2342,8 +2486,11 @@
       <c r="H46">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>25</v>
       </c>
@@ -2368,8 +2515,11 @@
       <c r="H47">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I47">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>70</v>
       </c>
@@ -2394,8 +2544,11 @@
       <c r="H48">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I48">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>70</v>
       </c>
@@ -2420,8 +2573,11 @@
       <c r="H49">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I49">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>70</v>
       </c>
@@ -2446,8 +2602,11 @@
       <c r="H50">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I50">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>72</v>
       </c>
@@ -2472,8 +2631,11 @@
       <c r="H51">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>74</v>
       </c>
@@ -2498,8 +2660,11 @@
       <c r="H52">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>76</v>
       </c>
@@ -2524,8 +2689,11 @@
       <c r="H53">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I53">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>10</v>
       </c>
@@ -2550,8 +2718,11 @@
       <c r="H54">
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I54">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>79</v>
       </c>
@@ -2576,8 +2747,11 @@
       <c r="H55">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I55">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>68</v>
       </c>
@@ -2602,8 +2776,11 @@
       <c r="H56">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I56">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>82</v>
       </c>
@@ -2628,8 +2805,11 @@
       <c r="H57">
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I57">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>82</v>
       </c>
@@ -2654,8 +2834,11 @@
       <c r="H58">
         <v>1</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>49</v>
       </c>
@@ -2680,8 +2863,11 @@
       <c r="H59">
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>85</v>
       </c>
@@ -2706,8 +2892,11 @@
       <c r="H60">
         <v>1</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I60">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>70</v>
       </c>
@@ -2732,8 +2921,11 @@
       <c r="H61">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I61">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>52</v>
       </c>
@@ -2758,8 +2950,11 @@
       <c r="H62">
         <v>1</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I62">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>60</v>
       </c>
@@ -2784,8 +2979,11 @@
       <c r="H63">
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I63">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>10</v>
       </c>
@@ -2809,6 +3007,9 @@
       </c>
       <c r="H64">
         <v>1</v>
+      </c>
+      <c r="I64">
+        <v>6</v>
       </c>
     </row>
     <row r="65" spans="5:5" x14ac:dyDescent="0.25">

</xml_diff>